<commit_message>
added App page 1
</commit_message>
<xml_diff>
--- a/media/Generated_Report_file.xlsx
+++ b/media/Generated_Report_file.xlsx
@@ -771,11 +771,11 @@
       <c r="C15" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Sat Jan 11 09:07:56.086 UTC
+Sat Jan 11 10:54:50.380 UTC
 ---- node0_RP0_CPU0 ----
 Memory information:
     Physical Memory     : 6144.0   MB
-    Free Memory         : 3548.792 MB
+    Free Memory         : 3548.386 MB
     Memory State        :   Normal
 </t>
         </is>
@@ -842,7 +842,7 @@
       <c r="C18" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Sat Jan 11 09:08:16.801 UTC
+Sat Jan 11 10:55:11.031 UTC
 controller Optics0/0/0/1
  description Scr1-Prot
  bits-per-symbol 3.4375
@@ -891,7 +891,7 @@
       <c r="C20" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Sat Jan 11 09:08:27.461 UTC</t>
+Sat Jan 11 10:55:21.715 UTC</t>
         </is>
       </c>
     </row>
@@ -957,12 +957,12 @@
       <c r="C23" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Sat Jan 11 09:08:48.128 UTC
+Sat Jan 11 10:55:42.390 UTC
 SSH version : Cisco-2.0 
 id       chan pty     location        state           userid    host                  ver authentication connection type
 -------------------------------------------------------------------------------------------------------------------------------
 Incoming sessions
-50200    1    vty1    0/RP0/CPU0      SESSION_OPEN    admin     10.110.195.179        v2  password       Command-Line-Interface 
+50479    1    vty0    0/RP0/CPU0      SESSION_OPEN    admin     10.110.195.179        v2  password       Command-Line-Interface 
 Outgoing sessions
 </t>
         </is>

</xml_diff>